<commit_message>
update Software Testing skill
</commit_message>
<xml_diff>
--- a/Deliverable-1/Skill Selection - Team D.xlsx
+++ b/Deliverable-1/Skill Selection - Team D.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/github_projects/SOEN-6011-TEAM-D/Deliverable-1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DFA1F5-17CE-B04A-80F2-22632514F089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -103,9 +112,6 @@
     <t>Software Testing Techniques</t>
   </si>
   <si>
-    <t>Automated Unit Testing, Test Driven Development</t>
-  </si>
-  <si>
     <t>Sareh</t>
   </si>
   <si>
@@ -149,39 +155,45 @@
   </si>
   <si>
     <t xml:space="preserve">Problem Analysis </t>
+  </si>
+  <si>
+    <t>Writing Unit Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -189,7 +201,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -204,8 +216,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="6">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -219,53 +237,115 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -455,28 +535,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.86"/>
-    <col customWidth="1" min="2" max="2" width="15.71"/>
-    <col customWidth="1" min="3" max="3" width="17.29"/>
-    <col customWidth="1" min="4" max="4" width="47.71"/>
-    <col customWidth="1" min="5" max="5" width="44.86"/>
-    <col customWidth="1" min="6" max="6" width="104.0"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" customWidth="1"/>
+    <col min="6" max="6" width="104" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -504,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>4.0104545E7</v>
+        <v>40104545</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -516,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -524,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3">
-        <v>4.0105186E7</v>
+        <v>40105186</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
@@ -536,7 +621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -544,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0084737E7</v>
+        <v>40084737</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
@@ -552,11 +637,11 @@
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -564,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="3">
-        <v>4.0103928E7</v>
+        <v>40103928</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>23</v>
@@ -572,11 +657,11 @@
       <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -584,79 +669,79 @@
         <v>27</v>
       </c>
       <c r="C6" s="3">
-        <v>4.0058782E7</v>
+        <v>40058782</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3">
+        <v>27845782</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3">
-        <v>2.7845782E7</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3">
+        <v>40042321</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3">
-        <v>4.0042321E7</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3">
+        <v>40085663</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3">
-        <v>4.0085663E7</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changing management skill to scheduling
</commit_message>
<xml_diff>
--- a/Deliverable-1/Skill Selection - Team D.xlsx
+++ b/Deliverable-1/Skill Selection - Team D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/github_projects/SOEN-6011-TEAM-D/Deliverable-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\GitHub\SOEN-6011-TEAM-D\Deliverable-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DFA1F5-17CE-B04A-80F2-22632514F089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C8674-F1F9-4A88-A2E2-E0E96BCEE933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Software Project Planning/Risk Management</t>
   </si>
   <si>
-    <t>Ability to Influence People</t>
-  </si>
-  <si>
     <t>Yash Chandreshkumar</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Writing Unit Testing</t>
+  </si>
+  <si>
+    <t>Scheduling</t>
   </si>
 </sst>
 </file>
@@ -548,20 +548,20 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
     <col min="6" max="6" width="104" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -641,7 +641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -661,7 +661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -678,10 +678,10 @@
         <v>29</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -701,7 +701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -718,27 +718,27 @@
         <v>38</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="3">
         <v>40085663</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Index is now Responsive
Using CSS the index on top of the skill pages is now responsive. Also the name of the skill has been updated in the excel file.
</commit_message>
<xml_diff>
--- a/Deliverable-1/Skill Selection - Team D.xlsx
+++ b/Deliverable-1/Skill Selection - Team D.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\GitHub\SOEN-6011-TEAM-D\Deliverable-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amin_\Documents\Sestopia\SOEN-6011-TEAM-D\Deliverable-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C8674-F1F9-4A88-A2E2-E0E96BCEE933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C56EA85-3B50-4AD5-9916-FBD24654DE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Requirements Specification</t>
   </si>
   <si>
-    <t>System Definition Document</t>
-  </si>
-  <si>
     <t>Rafael</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Scheduling</t>
+  </si>
+  <si>
+    <t>Software Requirements Elicitation</t>
   </si>
 </sst>
 </file>
@@ -551,17 +551,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" customWidth="1"/>
     <col min="6" max="6" width="104" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -641,7 +641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -661,7 +661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -678,10 +678,10 @@
         <v>29</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -698,47 +698,47 @@
         <v>33</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C8" s="3">
         <v>40042321</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C9" s="3">
         <v>40085663</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my skill name
</commit_message>
<xml_diff>
--- a/Deliverable-1/Skill Selection - Team D.xlsx
+++ b/Deliverable-1/Skill Selection - Team D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amin_\Documents\Sestopia\SOEN-6011-TEAM-D\Deliverable-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/Sestopia/SOEN-6011-TEAM-D/Deliverable-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C56EA85-3B50-4AD5-9916-FBD24654DE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D7DDF7-5ED1-D948-9F42-060B151DCB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,13 +151,13 @@
     <t xml:space="preserve">Problem Analysis </t>
   </si>
   <si>
-    <t>Writing Unit Testing</t>
-  </si>
-  <si>
     <t>Scheduling</t>
   </si>
   <si>
     <t>Software Requirements Elicitation</t>
+  </si>
+  <si>
+    <t>Automated Unit Testing</t>
   </si>
 </sst>
 </file>
@@ -547,21 +547,21 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" customWidth="1"/>
     <col min="6" max="6" width="104" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -641,7 +641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -661,7 +661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -678,10 +678,10 @@
         <v>29</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -698,10 +698,10 @@
         <v>33</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -718,10 +718,10 @@
         <v>37</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>

</xml_diff>